<commit_message>
Contributions Added (so far)
</commit_message>
<xml_diff>
--- a/Project Report/CSD2550_Contribution Formula_FinalSubmission (1).xlsx
+++ b/Project Report/CSD2550_Contribution Formula_FinalSubmission (1).xlsx
@@ -532,7 +532,7 @@
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -588,17 +588,17 @@
         <v>0</v>
       </c>
       <c r="D2" s="7">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="E2" s="7">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="F2" s="7">
         <v>0</v>
       </c>
       <c r="G2" t="str">
         <f>IF(SUM(D2:F2)&lt;&gt;1,IF(SUM(D2:F2)=0, "Not implemented", "Error"),"Ok")</f>
-        <v>Not implemented</v>
+        <v>Ok</v>
       </c>
       <c r="H2" s="2"/>
     </row>
@@ -613,7 +613,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="7">
         <v>0</v>
@@ -623,7 +623,7 @@
       </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G24" si="0">IF(SUM(D3:F3)&lt;&gt;1,IF(SUM(D3:F3)=0, "Not implemented", "Error"),"Ok")</f>
-        <v>Not implemented</v>
+        <v>Ok</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -644,11 +644,11 @@
         <v>0</v>
       </c>
       <c r="F4" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
-        <v>Not implemented</v>
+        <v>Ok</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -693,11 +693,11 @@
         <v>0</v>
       </c>
       <c r="F6" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>Not implemented</v>
+        <v>Ok</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -711,7 +711,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="7">
         <v>0</v>
@@ -721,7 +721,7 @@
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v>Not implemented</v>
+        <v>Ok</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -735,7 +735,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="7">
         <v>0</v>
@@ -745,7 +745,7 @@
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v>Not implemented</v>
+        <v>Ok</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -783,7 +783,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="7">
         <v>0</v>
@@ -793,7 +793,7 @@
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
-        <v>Not implemented</v>
+        <v>Ok</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -807,7 +807,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="7">
         <v>0</v>
@@ -817,7 +817,7 @@
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
-        <v>Not implemented</v>
+        <v>Ok</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -831,7 +831,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="7">
         <v>0</v>
@@ -841,7 +841,7 @@
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
-        <v>Not implemented</v>
+        <v>Ok</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -855,7 +855,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="7">
         <v>0</v>
@@ -865,7 +865,7 @@
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
-        <v>Not implemented</v>
+        <v>Ok</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -879,7 +879,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="7">
         <v>0</v>
@@ -889,7 +889,7 @@
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
-        <v>Not implemented</v>
+        <v>Ok</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -903,17 +903,17 @@
         <v>0</v>
       </c>
       <c r="D15" s="7">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="E15" s="7">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="F15" s="7">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
-        <v>Not implemented</v>
+        <v>Ok</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -927,17 +927,17 @@
         <v>0</v>
       </c>
       <c r="D16" s="7">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="E16" s="7">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="F16" s="7">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
-        <v>Not implemented</v>
+        <v>Ok</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1047,17 +1047,17 @@
         <v>0</v>
       </c>
       <c r="D21" s="7">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="E21" s="7">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="F21" s="7">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
-        <v>Not implemented</v>
+        <v>Ok</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1071,17 +1071,17 @@
         <v>0</v>
       </c>
       <c r="D22" s="7">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="E22" s="7">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="F22" s="7">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
-        <v>Not implemented</v>
+        <v>Ok</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Contributions Update - all Agreed
</commit_message>
<xml_diff>
--- a/Project Report/CSD2550_Contribution Formula_FinalSubmission (1).xlsx
+++ b/Project Report/CSD2550_Contribution Formula_FinalSubmission (1).xlsx
@@ -532,7 +532,7 @@
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -663,7 +663,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="7">
         <v>0</v>
@@ -673,7 +673,7 @@
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
-        <v>Not implemented</v>
+        <v>Ok</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -759,7 +759,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="7">
         <v>0</v>
@@ -769,7 +769,7 @@
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
-        <v>Not implemented</v>
+        <v>Ok</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -954,14 +954,14 @@
         <v>0</v>
       </c>
       <c r="E17" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="7">
         <v>0</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
-        <v>Not implemented</v>
+        <v>Ok</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -978,14 +978,14 @@
         <v>0</v>
       </c>
       <c r="E18" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="7">
         <v>0</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
-        <v>Not implemented</v>
+        <v>Ok</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1002,14 +1002,14 @@
         <v>0</v>
       </c>
       <c r="E19" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="7">
         <v>0</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
-        <v>Not implemented</v>
+        <v>Ok</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1026,14 +1026,14 @@
         <v>0</v>
       </c>
       <c r="E20" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="7">
         <v>0</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
-        <v>Not implemented</v>
+        <v>Ok</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1095,7 +1095,7 @@
         <v>0</v>
       </c>
       <c r="D23" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="7">
         <v>0</v>
@@ -1105,7 +1105,7 @@
       </c>
       <c r="G23" t="str">
         <f t="shared" si="0"/>
-        <v>Not implemented</v>
+        <v>Ok</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1119,7 +1119,7 @@
         <v>0</v>
       </c>
       <c r="D24" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="7">
         <v>0</v>
@@ -1129,7 +1129,7 @@
       </c>
       <c r="G24" t="str">
         <f t="shared" si="0"/>
-        <v>Not implemented</v>
+        <v>Ok</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>